<commit_message>
commit Code in extent branch with extent work
</commit_message>
<xml_diff>
--- a/src/main/java/excel/Navigate.xlsx
+++ b/src/main/java/excel/Navigate.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gagandeepsingh/IdeaProjects/ExcelPro/src/main/java/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gagandeepsingh/IdeaProjects/excelPro1/src/main/java/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="48">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -126,9 +126,6 @@
     <t>Qqqqq@1234</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
     <t>Click on Shop By Category Link</t>
   </si>
   <si>
@@ -171,13 +168,17 @@
     <t>Login</t>
   </si>
   <si>
-    <t>No</t>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -496,15 +497,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="31.1640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.1640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.69921875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -523,27 +525,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
         <v>35</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -555,17 +560,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="52.1640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="40.83203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.1640625" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="52.1640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="40.83203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.69921875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -593,7 +599,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -605,12 +611,12 @@
         <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -622,15 +628,15 @@
         <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -648,12 +654,12 @@
         <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -671,12 +677,12 @@
         <v>31</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -691,52 +697,52 @@
         <v>29</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
         <v>33</v>
-      </c>
-      <c r="D7" t="s">
-        <v>34</v>
       </c>
       <c r="E7" t="s">
         <v>29</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" t="s">
         <v>39</v>
       </c>
-      <c r="E8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" t="s">
-        <v>40</v>
-      </c>
       <c r="G8" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -747,10 +753,13 @@
       <c r="E9" t="s">
         <v>16</v>
       </c>
+      <c r="G9" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
@@ -762,15 +771,18 @@
         <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="G10" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
         <v>25</v>
@@ -784,13 +796,16 @@
       <c r="F11" t="s">
         <v>30</v>
       </c>
+      <c r="G11" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
         <v>26</v>
@@ -804,13 +819,16 @@
       <c r="F12" t="s">
         <v>31</v>
       </c>
+      <c r="G12" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
         <v>27</v>
@@ -821,39 +839,48 @@
       <c r="E13" t="s">
         <v>29</v>
       </c>
+      <c r="G13" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
         <v>33</v>
-      </c>
-      <c r="D14" t="s">
-        <v>34</v>
       </c>
       <c r="E14" t="s">
         <v>29</v>
       </c>
+      <c r="G14" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" t="s">
         <v>39</v>
       </c>
-      <c r="E15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" t="s">
-        <v>40</v>
+      <c r="G15" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>